<commit_message>
import for admin, labelling fixes
</commit_message>
<xml_diff>
--- a/public/assets/downloads/Member_import_template.xlsx
+++ b/public/assets/downloads/Member_import_template.xlsx
@@ -11,7 +11,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Instructions:
+1. Please read these instructions first to minimise potential errors during the data upload.
+2. Do not delete the row headings. Start from the row with the sample data (row 3).
+3. Email should be unique. If the email had already been saved before, the line will be ignored.
+4. Please fill in all data as correctly as possible
+5. Birthday should be in DATE format
+6. You can omit the RegionCode, ProvinceCode, and. CityCode. These will default to the Organisation’s values, but can be changed later in the system.
+7. Barangay refers to the Barangay where the member’s voting precinct is registered
+8. PositionInOrganisation refers to the Organisation you need to select in the dropdown when uploading the document in the system.
+9. IsRegisteredVoter should be either Y or N</t>
+  </si>
   <si>
     <t>FirstName</t>
   </si>
@@ -34,7 +46,7 @@
     <t>Barangay</t>
   </si>
   <si>
-    <t>Street</t>
+    <t>VotersID</t>
   </si>
   <si>
     <t>PositionInOrganisation</t>
@@ -82,7 +94,7 @@
     <t>Bgy I</t>
   </si>
   <si>
-    <t>JP Rizal</t>
+    <t>123-4455</t>
   </si>
   <si>
     <t>Student</t>
@@ -104,22 +116,30 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
+    <font/>
+    <font>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
       <b/>
+      <color rgb="FF999999"/>
     </font>
     <font>
       <b/>
       <sz val="9.0"/>
-      <color theme="1"/>
+      <color rgb="FF999999"/>
       <name val="Menlo"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -139,29 +159,41 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -376,7 +408,10 @@
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2.0" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B4" sqref="B4" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
@@ -398,104 +433,124 @@
     <col customWidth="1" min="17" max="17" width="9.71"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" ht="139.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3">
+      <c r="D3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="6">
         <v>9.191234567E9</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="F3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="G3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="H3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="I3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="5">
+      <c r="J3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="8">
         <v>30284.0</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="L3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="4">
+      <c r="M3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="7">
         <v>1000000.0</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
     <row r="5" ht="14.25" customHeight="1"/>
     <row r="6" ht="14.25" customHeight="1"/>
@@ -1432,10 +1487,10 @@
     <row r="937" ht="14.25" customHeight="1"/>
     <row r="938" ht="14.25" customHeight="1"/>
     <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>

</xml_diff>